<commit_message>
add/update for excel-to-json import payloads
</commit_message>
<xml_diff>
--- a/excel_to_Json_Converter_in_angularJS/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/excel_to_Json_Converter_in_angularJS/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC856093-CDD5-4AD2-990A-2C69EF20A9C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125D82DD-9A80-4527-BE62-8ACC6998FEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="1052">
   <si>
     <t>property</t>
   </si>
@@ -3560,7 +3560,7 @@
   <dimension ref="A1:F691"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3801,6 +3801,9 @@
       <c r="D13" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="E13" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -13301,18 +13304,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13513,18 +13516,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
update excel_to_Json_Converter_angularJS payload for dataValue/metadata
</commit_message>
<xml_diff>
--- a/excel_to_Json_Converter_in_angularJS/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/excel_to_Json_Converter_in_angularJS/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125D82DD-9A80-4527-BE62-8ACC6998FEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6096D9CF-D431-4CCA-B548-59449DFD48A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataElements" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2784" uniqueCount="1055">
   <si>
     <t>property</t>
   </si>
@@ -3187,6 +3187,15 @@
   </si>
   <si>
     <t>relationshipTypes</t>
+  </si>
+  <si>
+    <t>Burmese</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>programStages</t>
   </si>
 </sst>
 </file>
@@ -3557,10 +3566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6B5FAB-DF4A-42DC-8643-A674828EC12D}">
-  <dimension ref="A1:F691"/>
+  <dimension ref="A1:H691"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3572,7 +3581,7 @@
     <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3591,8 +3600,11 @@
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -3611,8 +3623,14 @@
       <c r="F2" s="2" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -3632,7 +3650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -3652,7 +3670,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -3669,7 +3687,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -3686,7 +3704,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -3703,7 +3721,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -3720,7 +3738,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -3734,10 +3752,10 @@
         <v>358</v>
       </c>
       <c r="E9" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -3754,7 +3772,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -3771,7 +3789,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -3788,7 +3806,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -3805,7 +3823,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -3819,7 +3837,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -3833,7 +3851,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -13304,18 +13322,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13516,18 +13534,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>